<commit_message>
Remove old publication files and regenerate JSON from Excel
Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/publications/my_publications.xlsx
+++ b/publications/my_publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manhara7\Documents\Workfiles\Homepage\angelikamanhart.github.io\angelikamanhart.github.io\publications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7DA93A-48C1-44ED-878E-8F1CC926B5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA89E9D6-0245-49CF-980C-56DBA65CCB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18900" yWindow="-3070" windowWidth="16200" windowHeight="9310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-12500" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="379">
   <si>
     <t>Type</t>
   </si>
@@ -1156,6 +1156,12 @@
   </si>
   <si>
     <t>publications/kinetic_myxobacteria_colonies_2021.pdf</t>
+  </si>
+  <si>
+    <t>Hartl B, Zeller I, Manhart A, Selitsch B, Lass-Floerl C, Willinger B</t>
+  </si>
+  <si>
+    <t>Manhart A,Windner SE,Baylies MK,Mogilner A</t>
   </si>
 </sst>
 </file>
@@ -1547,8 +1553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2298,7 +2304,7 @@
         <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>378</v>
       </c>
       <c r="E19" t="s">
         <v>168</v>
@@ -2637,7 +2643,7 @@
         <v>121</v>
       </c>
       <c r="D28" t="s">
-        <v>235</v>
+        <v>377</v>
       </c>
       <c r="E28" t="s">
         <v>236</v>

</xml_diff>

<commit_message>
Update site: redesign about links, reorder nav, add micro-macro tag, refine contact & outreach
- Restyle About section links as button-style (matching research page)
- Update bio interest tags and remove capitalization
- Reorder nav across all pages: About, Research, Publications, Outreach & Art, Team, CV, Contact
- Add micro-macro publication filter tag
- Replace contact emoji icons with SVG, update office/address, brighten email link
- Update outreach: WiS thumbnail, Rhythms card text & tags
- Remove duplicate/unused images
- Regenerate publications JSON

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/publications/my_publications.xlsx
+++ b/publications/my_publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manhara7\Documents\Workfiles\Homepage\angelikamanhart.github.io\angelikamanhart.github.io\publications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA89E9D6-0245-49CF-980C-56DBA65CCB2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3DB03A-4009-4FED-93C2-A5A3B72014C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-12500" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19120" yWindow="-6310" windowWidth="16200" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="380">
   <si>
     <t>Type</t>
   </si>
@@ -75,9 +75,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>collective; other</t>
-  </si>
-  <si>
     <t>Lancaster C, Manhart A, Pichaud F</t>
   </si>
   <si>
@@ -1162,6 +1159,12 @@
   </si>
   <si>
     <t>Manhart A,Windner SE,Baylies MK,Mogilner A</t>
+  </si>
+  <si>
+    <t>collective; micromacro</t>
+  </si>
+  <si>
+    <t>collective; bacteria; micromacro</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1619,16 +1622,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
       </c>
       <c r="G2">
         <v>2025</v>
@@ -1640,19 +1643,19 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.5">
@@ -1660,31 +1663,31 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
       </c>
       <c r="G3" s="1">
         <v>2024</v>
       </c>
       <c r="L3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.5">
@@ -1695,40 +1698,40 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>36</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>39</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.5">
@@ -1739,34 +1742,34 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>48</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>49</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>51</v>
-      </c>
-      <c r="N5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.5">
@@ -1777,28 +1780,28 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
       </c>
       <c r="G6" s="1">
         <v>2023</v>
       </c>
       <c r="L6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
         <v>57</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>58</v>
-      </c>
-      <c r="N6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.5">
@@ -1806,40 +1809,40 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>378</v>
       </c>
       <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
         <v>60</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>61</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" t="s">
         <v>63</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
         <v>64</v>
       </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>65</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>66</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>67</v>
-      </c>
-      <c r="N7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.5">
@@ -1847,31 +1850,31 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>70</v>
       </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1">
         <v>2022</v>
       </c>
       <c r="L8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" t="s">
         <v>72</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>73</v>
-      </c>
-      <c r="N8" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.5">
@@ -1882,37 +1885,37 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
         <v>75</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>77</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>79</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>80</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>81</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>82</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>83</v>
-      </c>
-      <c r="N9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.5">
@@ -1920,43 +1923,43 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
         <v>85</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>86</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" t="s">
         <v>88</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>89</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>90</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10" t="s">
         <v>91</v>
       </c>
-      <c r="K10" t="s">
-        <v>88</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>92</v>
       </c>
-      <c r="M10" t="s">
-        <v>93</v>
-      </c>
       <c r="N10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.5">
@@ -1964,40 +1967,40 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>378</v>
       </c>
       <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
         <v>94</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" t="s">
         <v>96</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>97</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>98</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>99</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>100</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>101</v>
-      </c>
-      <c r="N11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.5">
@@ -2008,40 +2011,40 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
         <v>103</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>104</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>105</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>107</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>108</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>109</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>111</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>112</v>
-      </c>
-      <c r="N12" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.5">
@@ -2052,34 +2055,34 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
         <v>114</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>115</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
         <v>116</v>
       </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>117</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>118</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>119</v>
-      </c>
-      <c r="N13" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.5">
@@ -2087,40 +2090,40 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
         <v>121</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>122</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>123</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" t="s">
         <v>125</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" t="s">
         <v>126</v>
       </c>
-      <c r="I14" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>127</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>128</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>129</v>
-      </c>
-      <c r="N14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.5">
@@ -2131,40 +2134,40 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" t="s">
         <v>131</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>132</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" t="s">
         <v>134</v>
       </c>
-      <c r="I15" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>135</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>136</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>137</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>138</v>
-      </c>
-      <c r="N15" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.5">
@@ -2175,34 +2178,34 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" t="s">
         <v>140</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
         <v>141</v>
       </c>
-      <c r="F16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="K16" t="s">
         <v>142</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>143</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>144</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>145</v>
-      </c>
-      <c r="N16" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.5">
@@ -2210,43 +2213,43 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
         <v>147</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>148</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" t="s">
         <v>150</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>151</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>152</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>153</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>154</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>155</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>156</v>
-      </c>
-      <c r="N17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.5">
@@ -2254,43 +2257,43 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>379</v>
       </c>
       <c r="D18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" t="s">
         <v>158</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>159</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>161</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>162</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
+        <v>153</v>
+      </c>
+      <c r="L18" t="s">
         <v>163</v>
       </c>
-      <c r="K18" t="s">
-        <v>154</v>
-      </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>164</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>165</v>
-      </c>
-      <c r="N18" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.5">
@@ -2301,31 +2304,31 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" t="s">
         <v>168</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" t="s">
         <v>169</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>170</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>171</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>172</v>
-      </c>
-      <c r="N19" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.5">
@@ -2336,40 +2339,40 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" t="s">
         <v>174</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>175</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H20" t="s">
         <v>176</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" t="s">
         <v>177</v>
       </c>
-      <c r="I20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>178</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>179</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>180</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>181</v>
-      </c>
-      <c r="N20" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.5">
@@ -2377,78 +2380,78 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>379</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" t="s">
         <v>183</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" t="s">
         <v>185</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>186</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>187</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
+        <v>184</v>
+      </c>
+      <c r="L21" t="s">
         <v>188</v>
       </c>
-      <c r="K21" t="s">
-        <v>185</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>189</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>190</v>
-      </c>
-      <c r="N21" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
         <v>192</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>193</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>194</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K22" t="s">
+        <v>184</v>
+      </c>
+      <c r="L22" t="s">
         <v>195</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K22" t="s">
-        <v>185</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>196</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>197</v>
-      </c>
-      <c r="N22" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.5">
@@ -2459,31 +2462,31 @@
         <v>15</v>
       </c>
       <c r="C23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D23" t="s">
         <v>199</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>200</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>201</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="K23" t="s">
         <v>203</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>204</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>205</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>206</v>
-      </c>
-      <c r="N23" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.5">
@@ -2491,34 +2494,34 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" t="s">
         <v>208</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>209</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K24" t="s">
         <v>210</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>211</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>212</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>213</v>
-      </c>
-      <c r="N24" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.5">
@@ -2526,34 +2529,34 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
+        <v>214</v>
+      </c>
+      <c r="E25" t="s">
         <v>215</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>209</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K25" t="s">
+        <v>210</v>
+      </c>
+      <c r="L25" t="s">
         <v>216</v>
       </c>
-      <c r="F25" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K25" t="s">
-        <v>211</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>217</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>218</v>
-      </c>
-      <c r="N25" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.5">
@@ -2561,34 +2564,34 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E26" t="s">
+        <v>219</v>
+      </c>
+      <c r="F26" t="s">
         <v>220</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="K26" t="s">
         <v>222</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>223</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>224</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>225</v>
-      </c>
-      <c r="N26" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.5">
@@ -2599,37 +2602,37 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" t="s">
         <v>227</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>228</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" t="s">
+        <v>88</v>
+      </c>
+      <c r="I27" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" t="s">
         <v>230</v>
       </c>
-      <c r="H27" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" t="s">
-        <v>90</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>231</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>232</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>233</v>
-      </c>
-      <c r="N27" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.5">
@@ -2640,31 +2643,31 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E28" t="s">
+        <v>235</v>
+      </c>
+      <c r="F28" t="s">
         <v>236</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K28" t="s">
+        <v>169</v>
+      </c>
+      <c r="L28" t="s">
         <v>237</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K28" t="s">
-        <v>170</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>238</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>239</v>
-      </c>
-      <c r="N28" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2695,426 +2698,426 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
         <v>241</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>242</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>243</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>244</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>245</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>246</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>247</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>248</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>249</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>250</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>251</v>
-      </c>
-      <c r="L1" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" t="s">
         <v>253</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>254</v>
-      </c>
-      <c r="C2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" t="s">
         <v>256</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>257</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>258</v>
       </c>
-      <c r="E3" t="s">
-        <v>259</v>
-      </c>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s">
         <v>253</v>
       </c>
-      <c r="B4" t="s">
-        <v>254</v>
-      </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" t="s">
         <v>260</v>
-      </c>
-      <c r="B5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
         <v>262</v>
       </c>
-      <c r="B6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>263</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>264</v>
-      </c>
-      <c r="E6" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" t="s">
         <v>266</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>267</v>
       </c>
-      <c r="D7" t="s">
-        <v>268</v>
-      </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" t="s">
         <v>269</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" t="s">
         <v>270</v>
-      </c>
-      <c r="C8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" t="s">
         <v>272</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" t="s">
         <v>262</v>
       </c>
-      <c r="C9" t="s">
-        <v>273</v>
-      </c>
-      <c r="D9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>263</v>
-      </c>
-      <c r="F9" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" t="s">
         <v>274</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>275</v>
-      </c>
-      <c r="D10" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" t="s">
         <v>277</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" t="s">
         <v>278</v>
       </c>
-      <c r="C11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>279</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>275</v>
+      </c>
+      <c r="G11" t="s">
         <v>280</v>
-      </c>
-      <c r="F11" t="s">
-        <v>276</v>
-      </c>
-      <c r="G11" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" t="s">
         <v>282</v>
       </c>
-      <c r="B12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>283</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>284</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>285</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>286</v>
-      </c>
-      <c r="G12" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
         <v>288</v>
       </c>
-      <c r="B13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E13" t="s">
         <v>289</v>
-      </c>
-      <c r="D13" t="s">
-        <v>276</v>
-      </c>
-      <c r="E13" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" t="s">
         <v>291</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>292</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>293</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>294</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>295</v>
       </c>
-      <c r="G14" t="s">
-        <v>296</v>
-      </c>
       <c r="H14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" t="s">
         <v>275</v>
-      </c>
-      <c r="D17" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D20" t="s">
         <v>299</v>
-      </c>
-      <c r="C20" t="s">
-        <v>271</v>
-      </c>
-      <c r="D20" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24" t="s">
         <v>299</v>
-      </c>
-      <c r="C24" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
+        <v>301</v>
+      </c>
+      <c r="B25" t="s">
         <v>302</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>303</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>304</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>305</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>306</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>307</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>308</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" t="s">
         <v>309</v>
       </c>
-      <c r="I25" t="s">
-        <v>147</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>310</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>311</v>
-      </c>
-      <c r="L25" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
+        <v>312</v>
+      </c>
+      <c r="B26" t="s">
         <v>313</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>254</v>
+      </c>
+      <c r="D26" t="s">
         <v>314</v>
       </c>
-      <c r="C26" t="s">
-        <v>255</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>315</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>316</v>
-      </c>
-      <c r="F26" t="s">
-        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3157,52 +3160,52 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>3</v>
@@ -3211,7 +3214,7 @@
         <v>5</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>7</v>
@@ -3223,7 +3226,7 @@
         <v>9</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>11</v>
@@ -3231,25 +3234,25 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2" t="s">
-        <v>254</v>
-      </c>
-      <c r="F2" t="s">
-        <v>147</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
       </c>
       <c r="T2" s="1">
         <v>2024</v>
@@ -3257,146 +3260,146 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G3" t="s">
+        <v>257</v>
+      </c>
+      <c r="H3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+      <c r="R3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
-        <v>336</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G3" t="s">
-        <v>258</v>
-      </c>
-      <c r="H3" t="s">
-        <v>259</v>
-      </c>
-      <c r="I3" t="s">
-        <v>147</v>
-      </c>
-      <c r="R3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" t="s">
         <v>36</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>37</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>38</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" t="s">
+        <v>260</v>
+      </c>
+      <c r="R4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>260</v>
-      </c>
-      <c r="E4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F4" t="s">
-        <v>261</v>
-      </c>
-      <c r="R4" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="T4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" t="s">
         <v>47</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>48</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>49</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" t="s">
+        <v>337</v>
+      </c>
+      <c r="G5" t="s">
+        <v>338</v>
+      </c>
+      <c r="H5" t="s">
+        <v>252</v>
+      </c>
+      <c r="I5" t="s">
+        <v>339</v>
+      </c>
+      <c r="J5" t="s">
+        <v>340</v>
+      </c>
+      <c r="K5" t="s">
+        <v>341</v>
+      </c>
+      <c r="L5" t="s">
+        <v>342</v>
+      </c>
+      <c r="M5" t="s">
+        <v>343</v>
+      </c>
+      <c r="N5" t="s">
+        <v>344</v>
+      </c>
+      <c r="O5" t="s">
+        <v>146</v>
+      </c>
+      <c r="P5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>258</v>
+      </c>
+      <c r="S5" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E5" t="s">
-        <v>257</v>
-      </c>
-      <c r="F5" t="s">
-        <v>338</v>
-      </c>
-      <c r="G5" t="s">
-        <v>339</v>
-      </c>
-      <c r="H5" t="s">
-        <v>253</v>
-      </c>
-      <c r="I5" t="s">
-        <v>340</v>
-      </c>
-      <c r="J5" t="s">
-        <v>341</v>
-      </c>
-      <c r="K5" t="s">
-        <v>342</v>
-      </c>
-      <c r="L5" t="s">
-        <v>343</v>
-      </c>
-      <c r="M5" t="s">
-        <v>344</v>
-      </c>
-      <c r="N5" t="s">
-        <v>345</v>
-      </c>
-      <c r="O5" t="s">
-        <v>147</v>
-      </c>
-      <c r="P5" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>259</v>
-      </c>
-      <c r="S5" t="s">
-        <v>56</v>
       </c>
       <c r="T5" s="1">
         <v>2023</v>
@@ -3404,75 +3407,75 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G6" t="s">
+        <v>263</v>
+      </c>
+      <c r="H6" t="s">
+        <v>264</v>
+      </c>
+      <c r="R6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" t="s">
-        <v>346</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H6" t="s">
-        <v>265</v>
-      </c>
-      <c r="R6" t="s">
-        <v>60</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" t="s">
         <v>63</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
+        <v>47</v>
+      </c>
+      <c r="X6" t="s">
         <v>64</v>
       </c>
-      <c r="V6" t="s">
-        <v>48</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>65</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
+        <v>346</v>
+      </c>
+      <c r="E7" t="s">
         <v>347</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" t="s">
         <v>348</v>
       </c>
-      <c r="F7" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>349</v>
       </c>
-      <c r="H7" t="s">
-        <v>350</v>
-      </c>
       <c r="S7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T7" s="1">
         <v>2022</v>
@@ -3480,891 +3483,891 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H8" t="s">
+        <v>146</v>
+      </c>
+      <c r="R8" t="s">
+        <v>75</v>
+      </c>
+      <c r="S8" t="s">
         <v>77</v>
       </c>
-      <c r="B8" t="s">
-        <v>351</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" t="s">
-        <v>266</v>
-      </c>
-      <c r="F8" t="s">
-        <v>267</v>
-      </c>
-      <c r="G8" t="s">
-        <v>268</v>
-      </c>
-      <c r="H8" t="s">
-        <v>147</v>
-      </c>
-      <c r="R8" t="s">
-        <v>76</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>79</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>80</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>81</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
+        <v>351</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E9" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" t="s">
+        <v>270</v>
+      </c>
+      <c r="R9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" t="s">
         <v>86</v>
       </c>
-      <c r="B9" t="s">
-        <v>352</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E9" t="s">
-        <v>270</v>
-      </c>
-      <c r="F9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G9" t="s">
-        <v>271</v>
-      </c>
-      <c r="R9" t="s">
-        <v>85</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="T9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="U9" t="s">
         <v>88</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>89</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>90</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y9" t="s">
         <v>91</v>
-      </c>
-      <c r="X9" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F10" t="s">
+        <v>272</v>
+      </c>
+      <c r="G10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" t="s">
+        <v>262</v>
+      </c>
+      <c r="I10" t="s">
+        <v>263</v>
+      </c>
+      <c r="R10" t="s">
+        <v>93</v>
+      </c>
+      <c r="S10" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
-        <v>353</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>272</v>
-      </c>
-      <c r="E10" t="s">
-        <v>262</v>
-      </c>
-      <c r="F10" t="s">
-        <v>273</v>
-      </c>
-      <c r="G10" t="s">
-        <v>147</v>
-      </c>
-      <c r="H10" t="s">
-        <v>263</v>
-      </c>
-      <c r="I10" t="s">
-        <v>264</v>
-      </c>
-      <c r="R10" t="s">
-        <v>94</v>
-      </c>
-      <c r="S10" t="s">
-        <v>29</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" t="s">
         <v>96</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>97</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>98</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>99</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>353</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" t="s">
+        <v>273</v>
+      </c>
+      <c r="F11" t="s">
+        <v>289</v>
+      </c>
+      <c r="G11" t="s">
+        <v>275</v>
+      </c>
+      <c r="R11" t="s">
+        <v>354</v>
+      </c>
+      <c r="S11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" t="s">
-        <v>354</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E11" t="s">
-        <v>274</v>
-      </c>
-      <c r="F11" t="s">
-        <v>290</v>
-      </c>
-      <c r="G11" t="s">
-        <v>276</v>
-      </c>
-      <c r="R11" t="s">
-        <v>355</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="T11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U11" t="s">
         <v>106</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>107</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>108</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>109</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>110</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>355</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" t="s">
+        <v>278</v>
+      </c>
+      <c r="H12" t="s">
+        <v>279</v>
+      </c>
+      <c r="I12" t="s">
+        <v>275</v>
+      </c>
+      <c r="J12" t="s">
+        <v>280</v>
+      </c>
+      <c r="R12" t="s">
+        <v>114</v>
+      </c>
+      <c r="S12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U12" t="s">
+        <v>63</v>
+      </c>
+      <c r="X12" t="s">
         <v>116</v>
       </c>
-      <c r="B12" t="s">
-        <v>356</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>277</v>
-      </c>
-      <c r="E12" t="s">
-        <v>278</v>
-      </c>
-      <c r="F12" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" t="s">
-        <v>279</v>
-      </c>
-      <c r="H12" t="s">
-        <v>280</v>
-      </c>
-      <c r="I12" t="s">
-        <v>276</v>
-      </c>
-      <c r="J12" t="s">
-        <v>281</v>
-      </c>
-      <c r="R12" t="s">
-        <v>115</v>
-      </c>
-      <c r="S12" t="s">
-        <v>46</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="U12" t="s">
-        <v>64</v>
-      </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>117</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>281</v>
+      </c>
+      <c r="E13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" t="s">
+        <v>284</v>
+      </c>
+      <c r="I13" t="s">
+        <v>285</v>
+      </c>
+      <c r="J13" t="s">
+        <v>286</v>
+      </c>
+      <c r="R13" t="s">
+        <v>121</v>
+      </c>
+      <c r="S13" t="s">
         <v>123</v>
       </c>
-      <c r="B13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>282</v>
-      </c>
-      <c r="E13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F13" t="s">
-        <v>283</v>
-      </c>
-      <c r="G13" t="s">
-        <v>284</v>
-      </c>
-      <c r="H13" t="s">
-        <v>285</v>
-      </c>
-      <c r="I13" t="s">
-        <v>286</v>
-      </c>
-      <c r="J13" t="s">
-        <v>287</v>
-      </c>
-      <c r="R13" t="s">
-        <v>122</v>
-      </c>
-      <c r="S13" t="s">
+      <c r="T13" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="U13" t="s">
         <v>125</v>
       </c>
-      <c r="U13" t="s">
+      <c r="V13" t="s">
+        <v>47</v>
+      </c>
+      <c r="X13" t="s">
         <v>126</v>
       </c>
-      <c r="V13" t="s">
-        <v>48</v>
-      </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>127</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" t="s">
+        <v>288</v>
+      </c>
+      <c r="G14" t="s">
+        <v>275</v>
+      </c>
+      <c r="H14" t="s">
+        <v>289</v>
+      </c>
+      <c r="R14" t="s">
+        <v>130</v>
+      </c>
+      <c r="S14" t="s">
         <v>132</v>
       </c>
-      <c r="B14" t="s">
-        <v>358</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
-        <v>288</v>
-      </c>
-      <c r="E14" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" t="s">
-        <v>289</v>
-      </c>
-      <c r="G14" t="s">
-        <v>276</v>
-      </c>
-      <c r="H14" t="s">
-        <v>290</v>
-      </c>
-      <c r="R14" t="s">
-        <v>131</v>
-      </c>
-      <c r="S14" t="s">
+      <c r="T14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U14" t="s">
         <v>133</v>
       </c>
-      <c r="T14" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="U14" t="s">
+      <c r="V14" t="s">
+        <v>89</v>
+      </c>
+      <c r="W14" t="s">
         <v>134</v>
       </c>
-      <c r="V14" t="s">
-        <v>90</v>
-      </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>135</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Y14" t="s">
         <v>136</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
+        <v>358</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" t="s">
+        <v>290</v>
+      </c>
+      <c r="F15" t="s">
+        <v>291</v>
+      </c>
+      <c r="G15" t="s">
+        <v>292</v>
+      </c>
+      <c r="H15" t="s">
+        <v>293</v>
+      </c>
+      <c r="I15" t="s">
+        <v>294</v>
+      </c>
+      <c r="J15" t="s">
+        <v>295</v>
+      </c>
+      <c r="K15" t="s">
+        <v>275</v>
+      </c>
+      <c r="R15" t="s">
+        <v>139</v>
+      </c>
+      <c r="S15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U15" t="s">
         <v>141</v>
       </c>
-      <c r="B15" t="s">
-        <v>359</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E15" t="s">
-        <v>291</v>
-      </c>
-      <c r="F15" t="s">
-        <v>292</v>
-      </c>
-      <c r="G15" t="s">
-        <v>293</v>
-      </c>
-      <c r="H15" t="s">
-        <v>294</v>
-      </c>
-      <c r="I15" t="s">
-        <v>295</v>
-      </c>
-      <c r="J15" t="s">
-        <v>296</v>
-      </c>
-      <c r="K15" t="s">
-        <v>276</v>
-      </c>
-      <c r="R15" t="s">
-        <v>140</v>
-      </c>
-      <c r="S15" t="s">
-        <v>46</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="U15" t="s">
+      <c r="X15" t="s">
         <v>142</v>
       </c>
-      <c r="X15" t="s">
+      <c r="Y15" t="s">
         <v>143</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16" t="s">
+        <v>359</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>146</v>
+      </c>
+      <c r="R16" t="s">
+        <v>146</v>
+      </c>
+      <c r="S16" t="s">
         <v>148</v>
       </c>
-      <c r="B16" t="s">
-        <v>360</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>147</v>
-      </c>
-      <c r="R16" t="s">
-        <v>147</v>
-      </c>
-      <c r="S16" t="s">
+      <c r="T16" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="U16" t="s">
         <v>150</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>151</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>152</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>153</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>154</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>360</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" t="s">
+        <v>296</v>
+      </c>
+      <c r="R17" t="s">
+        <v>157</v>
+      </c>
+      <c r="S17" t="s">
         <v>159</v>
       </c>
-      <c r="B17" t="s">
-        <v>361</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>262</v>
-      </c>
-      <c r="E17" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" t="s">
-        <v>297</v>
-      </c>
-      <c r="R17" t="s">
-        <v>158</v>
-      </c>
-      <c r="S17" t="s">
+      <c r="T17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="U17" t="s">
         <v>160</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="U17" t="s">
+      <c r="V17" t="s">
         <v>161</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>162</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y17" t="s">
         <v>163</v>
-      </c>
-      <c r="X17" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F18" t="s">
+        <v>289</v>
+      </c>
+      <c r="G18" t="s">
+        <v>275</v>
+      </c>
+      <c r="R18" t="s">
+        <v>166</v>
+      </c>
+      <c r="S18" t="s">
         <v>168</v>
       </c>
-      <c r="B18" t="s">
-        <v>362</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E18" t="s">
-        <v>288</v>
-      </c>
-      <c r="F18" t="s">
-        <v>290</v>
-      </c>
-      <c r="G18" t="s">
-        <v>276</v>
-      </c>
-      <c r="R18" t="s">
-        <v>167</v>
-      </c>
-      <c r="S18" t="s">
+      <c r="T18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X18" t="s">
         <v>169</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>170</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>362</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>275</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="R19" t="s">
+        <v>173</v>
+      </c>
+      <c r="S19" t="s">
         <v>175</v>
       </c>
-      <c r="B19" t="s">
-        <v>363</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" t="s">
-        <v>147</v>
-      </c>
-      <c r="R19" t="s">
-        <v>174</v>
-      </c>
-      <c r="S19" t="s">
+      <c r="T19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="U19" t="s">
         <v>176</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
+        <v>89</v>
+      </c>
+      <c r="W19" t="s">
         <v>177</v>
       </c>
-      <c r="V19" t="s">
-        <v>90</v>
-      </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
         <v>178</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>179</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s">
+        <v>363</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" t="s">
+        <v>296</v>
+      </c>
+      <c r="R20" t="s">
+        <v>157</v>
+      </c>
+      <c r="S20" t="s">
         <v>183</v>
       </c>
-      <c r="B20" t="s">
-        <v>364</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>262</v>
-      </c>
-      <c r="E20" t="s">
-        <v>147</v>
-      </c>
-      <c r="F20" t="s">
-        <v>297</v>
-      </c>
-      <c r="R20" t="s">
-        <v>158</v>
-      </c>
-      <c r="S20" t="s">
+      <c r="T20" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="U20" t="s">
         <v>185</v>
       </c>
-      <c r="U20" t="s">
+      <c r="V20" t="s">
         <v>186</v>
       </c>
-      <c r="V20" t="s">
+      <c r="W20" t="s">
         <v>187</v>
       </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y20" t="s">
         <v>188</v>
-      </c>
-      <c r="X20" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>298</v>
+      </c>
+      <c r="F21" t="s">
+        <v>270</v>
+      </c>
+      <c r="G21" t="s">
+        <v>299</v>
+      </c>
+      <c r="R21" t="s">
+        <v>192</v>
+      </c>
+      <c r="S21" t="s">
         <v>194</v>
       </c>
-      <c r="B21" t="s">
-        <v>365</v>
-      </c>
-      <c r="C21" t="s">
-        <v>192</v>
-      </c>
-      <c r="D21" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" t="s">
-        <v>299</v>
-      </c>
-      <c r="F21" t="s">
-        <v>271</v>
-      </c>
-      <c r="G21" t="s">
-        <v>300</v>
-      </c>
-      <c r="R21" t="s">
-        <v>193</v>
-      </c>
-      <c r="S21" t="s">
+      <c r="T21" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X21" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y21" t="s">
         <v>195</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="X21" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" t="s">
+        <v>365</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" t="s">
+        <v>275</v>
+      </c>
+      <c r="R22" t="s">
+        <v>199</v>
+      </c>
+      <c r="S22" t="s">
         <v>201</v>
       </c>
-      <c r="B22" t="s">
-        <v>366</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" t="s">
-        <v>276</v>
-      </c>
-      <c r="R22" t="s">
-        <v>200</v>
-      </c>
-      <c r="S22" t="s">
+      <c r="T22" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="X22" t="s">
         <v>203</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>204</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" t="s">
+        <v>366</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E23" t="s">
+        <v>270</v>
+      </c>
+      <c r="R23" t="s">
+        <v>207</v>
+      </c>
+      <c r="S23" t="s">
         <v>209</v>
       </c>
-      <c r="B23" t="s">
-        <v>367</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>147</v>
-      </c>
-      <c r="E23" t="s">
-        <v>271</v>
-      </c>
-      <c r="R23" t="s">
-        <v>208</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="T23" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X23" t="s">
         <v>210</v>
       </c>
-      <c r="T23" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>211</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
+        <v>300</v>
+      </c>
+      <c r="E24" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" t="s">
+        <v>270</v>
+      </c>
+      <c r="R24" t="s">
+        <v>214</v>
+      </c>
+      <c r="S24" t="s">
+        <v>209</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X24" t="s">
+        <v>210</v>
+      </c>
+      <c r="Y24" t="s">
         <v>216</v>
-      </c>
-      <c r="B24" t="s">
-        <v>368</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>301</v>
-      </c>
-      <c r="E24" t="s">
-        <v>147</v>
-      </c>
-      <c r="F24" t="s">
-        <v>271</v>
-      </c>
-      <c r="R24" t="s">
-        <v>215</v>
-      </c>
-      <c r="S24" t="s">
-        <v>210</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="X24" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
+        <v>368</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" t="s">
+        <v>298</v>
+      </c>
+      <c r="F25" t="s">
+        <v>270</v>
+      </c>
+      <c r="G25" t="s">
+        <v>299</v>
+      </c>
+      <c r="R25" t="s">
+        <v>192</v>
+      </c>
+      <c r="S25" t="s">
         <v>220</v>
       </c>
-      <c r="B25" t="s">
-        <v>369</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" t="s">
-        <v>299</v>
-      </c>
-      <c r="F25" t="s">
-        <v>271</v>
-      </c>
-      <c r="G25" t="s">
-        <v>300</v>
-      </c>
-      <c r="R25" t="s">
-        <v>193</v>
-      </c>
-      <c r="S25" t="s">
+      <c r="T25" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="X25" t="s">
         <v>222</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>223</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
+        <v>301</v>
+      </c>
+      <c r="E26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F26" t="s">
+        <v>303</v>
+      </c>
+      <c r="G26" t="s">
+        <v>304</v>
+      </c>
+      <c r="H26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I26" t="s">
+        <v>306</v>
+      </c>
+      <c r="J26" t="s">
+        <v>307</v>
+      </c>
+      <c r="K26" t="s">
+        <v>308</v>
+      </c>
+      <c r="L26" t="s">
+        <v>146</v>
+      </c>
+      <c r="M26" t="s">
+        <v>309</v>
+      </c>
+      <c r="N26" t="s">
+        <v>310</v>
+      </c>
+      <c r="O26" t="s">
+        <v>311</v>
+      </c>
+      <c r="R26" t="s">
+        <v>226</v>
+      </c>
+      <c r="S26" t="s">
         <v>228</v>
       </c>
-      <c r="B26" t="s">
-        <v>370</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" t="s">
-        <v>302</v>
-      </c>
-      <c r="E26" t="s">
-        <v>303</v>
-      </c>
-      <c r="F26" t="s">
-        <v>304</v>
-      </c>
-      <c r="G26" t="s">
-        <v>305</v>
-      </c>
-      <c r="H26" t="s">
-        <v>306</v>
-      </c>
-      <c r="I26" t="s">
-        <v>307</v>
-      </c>
-      <c r="J26" t="s">
-        <v>308</v>
-      </c>
-      <c r="K26" t="s">
-        <v>309</v>
-      </c>
-      <c r="L26" t="s">
-        <v>147</v>
-      </c>
-      <c r="M26" t="s">
-        <v>310</v>
-      </c>
-      <c r="N26" t="s">
-        <v>311</v>
-      </c>
-      <c r="O26" t="s">
-        <v>312</v>
-      </c>
-      <c r="R26" t="s">
-        <v>227</v>
-      </c>
-      <c r="S26" t="s">
+      <c r="T26" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="T26" s="1" t="s">
+      <c r="U26" t="s">
+        <v>88</v>
+      </c>
+      <c r="V26" t="s">
+        <v>89</v>
+      </c>
+      <c r="X26" t="s">
         <v>230</v>
       </c>
-      <c r="U26" t="s">
-        <v>89</v>
-      </c>
-      <c r="V26" t="s">
-        <v>90</v>
-      </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>231</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
+        <v>235</v>
+      </c>
+      <c r="B27" t="s">
+        <v>370</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>312</v>
+      </c>
+      <c r="E27" t="s">
+        <v>371</v>
+      </c>
+      <c r="F27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" t="s">
+        <v>372</v>
+      </c>
+      <c r="H27" t="s">
+        <v>373</v>
+      </c>
+      <c r="I27" t="s">
+        <v>374</v>
+      </c>
+      <c r="R27" t="s">
+        <v>234</v>
+      </c>
+      <c r="S27" t="s">
         <v>236</v>
       </c>
-      <c r="B27" t="s">
-        <v>371</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>313</v>
-      </c>
-      <c r="E27" t="s">
-        <v>372</v>
-      </c>
-      <c r="F27" t="s">
-        <v>147</v>
-      </c>
-      <c r="G27" t="s">
-        <v>373</v>
-      </c>
-      <c r="H27" t="s">
-        <v>374</v>
-      </c>
-      <c r="I27" t="s">
-        <v>375</v>
-      </c>
-      <c r="R27" t="s">
-        <v>235</v>
-      </c>
-      <c r="S27" t="s">
+      <c r="T27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X27" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y27" t="s">
         <v>237</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="X27" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redesign site: CV edits, file reorganization, cleanup, and UI improvements
- CV: add Study Break label, "With" prefix on mentors, split Assist/Assoc Professor with dividers
- Hero: simplify tagline text
- About: fix i_knew image overflow on narrow screens, update path
- Publications: change micro-macro tag color, disable node drag in non-edit mode, scroll to list on click, add legend hint
- Outreach: rename section headings, reorder sections, move sub-pages into outreach/
- Research: add Winkler 2024 publication to MOHECCE, rename Experimental Component, adjust subtitle line breaks
- Contact: obfuscate email with char codes
- Reorganize file structure into section-based folders (shared/, cv/, research/, outreach/, team/, maintenance/)
- Remove orphaned pages (teaching, research_map, coauthorship_network, cv_journey_map) and unused assets
- Fix imerpial→imperial filename typo

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/publications/my_publications.xlsx
+++ b/publications/my_publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manhara7\Documents\Workfiles\Homepage\angelikamanhart.github.io\angelikamanhart.github.io\publications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3DB03A-4009-4FED-93C2-A5A3B72014C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F22CF1E-B298-4542-A55D-A8543C707B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19120" yWindow="-6310" windowWidth="16200" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23160" yWindow="-6310" windowWidth="20240" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="1" r:id="rId1"/>
@@ -1557,7 +1557,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1926,7 +1926,7 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>379</v>
       </c>
       <c r="D10" t="s">
         <v>84</v>

</xml_diff>